<commit_message>
Modifica Moral Resico acumulado IRS
</commit_message>
<xml_diff>
--- a/tablas_sistema.xlsx
+++ b/tablas_sistema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dtax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09351153-94F5-4691-A1E6-88F07929C05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC258BF-C953-4812-895E-8B849798292B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="503">
   <si>
     <t>Structure for</t>
   </si>
@@ -2243,7 +2243,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2347,7 +2347,6 @@
     <xf numFmtId="0" fontId="27" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="17" fillId="46" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7495,8 +7494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046B3F70-AF4F-4F89-A5C8-9E1487C489FC}">
   <dimension ref="A2:AP54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA28" workbookViewId="0">
-      <selection activeCell="AL39" sqref="AL39"/>
+    <sheetView tabSelected="1" topLeftCell="T16" workbookViewId="0">
+      <selection activeCell="AC47" sqref="AC47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9812,8 +9811,8 @@
       <c r="AF37" t="s">
         <v>487</v>
       </c>
-      <c r="AI37" s="35">
-        <v>38</v>
+      <c r="AI37" s="35" t="s">
+        <v>492</v>
       </c>
       <c r="AJ37" t="s">
         <v>495</v>
@@ -10028,7 +10027,7 @@
       <c r="AF41" t="s">
         <v>480</v>
       </c>
-      <c r="AI41" s="51">
+      <c r="AI41" s="35">
         <v>41</v>
       </c>
       <c r="AJ41" t="s">
@@ -10078,7 +10077,7 @@
       <c r="AF42" t="s">
         <v>481</v>
       </c>
-      <c r="AI42" s="51">
+      <c r="AI42" s="35">
         <v>42</v>
       </c>
       <c r="AJ42" t="s">

</xml_diff>